<commit_message>
Added one more scenario
</commit_message>
<xml_diff>
--- a/Testdata/Non_Oncology/DataFiles/LiveSLRPage/NonOnco_SLRReport_Data.xlsx
+++ b/Testdata/Non_Oncology/DataFiles/LiveSLRPage/NonOnco_SLRReport_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VersionControl\pse.autotest\Testdata\Non_Oncology\DataFiles\LiveSLRPage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{812F467E-6A38-41AE-B52A-E1157FE6127C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F22E9C5-D4EE-4C80-A5C1-62BD122AB9AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{26C09FF1-B3A3-4547-AFE4-A3356FE600D6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{26C09FF1-B3A3-4547-AFE4-A3356FE600D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
   <si>
     <t>Name</t>
   </si>
@@ -104,9 +104,6 @@
     <t>study_design_section</t>
   </si>
   <si>
-    <t>ExpectedSourceTemplateFile_Excel</t>
-  </si>
-  <si>
     <t>\Testdata\Non_Oncology\Templates\SLRReport_SourceData\NonOnco_Expected_TestData.xlsx</t>
   </si>
   <si>
@@ -117,6 +114,24 @@
   </si>
   <si>
     <t>ExpectedFilenames</t>
+  </si>
+  <si>
+    <t>scenario2</t>
+  </si>
+  <si>
+    <t>reported_variable_section</t>
+  </si>
+  <si>
+    <t>\Testdata\Non_Oncology\Templates\SLRReport_SourceData\NonOnco_Expected_TestData_with_filters.xlsx</t>
+  </si>
+  <si>
+    <t>reported_variable_section3</t>
+  </si>
+  <si>
+    <t>reported_variable_section3_checkbox</t>
+  </si>
+  <si>
+    <t>ExpectedSourceTemplateFile</t>
   </si>
 </sst>
 </file>
@@ -477,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{344B1479-70F0-4B4E-BC73-42393FEE027A}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -489,10 +504,10 @@
     <col min="3" max="3" width="60.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="81.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="92" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="79.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -522,10 +537,10 @@
         <v>12</v>
       </c>
       <c r="I1" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="J1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -544,51 +559,95 @@
       <c r="E2" t="s">
         <v>9</v>
       </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" t="s">
-        <v>15</v>
-      </c>
       <c r="I2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" t="s">
         <v>23</v>
-      </c>
-      <c r="J2" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="F3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" t="s">
-        <v>18</v>
-      </c>
       <c r="J3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="F4" t="s">
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" t="s">
         <v>19</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G8" t="s">
         <v>20</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H8" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" t="s">
+        <v>30</v>
+      </c>
+      <c r="H9" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>